<commit_message>
Added command to insert blank line after cursor row.
'MoveRows' command.
</commit_message>
<xml_diff>
--- a/docs/character-codes.xlsx
+++ b/docs/character-codes.xlsx
@@ -3333,7 +3333,7 @@
     <t xml:space="preserve">CMD_INSTOG</t>
   </si>
   <si>
-    <t xml:space="preserve">Toggles insert mode.</t>
+    <t xml:space="preserve">Toggles insert mode. In inset mode, new characters are inserted at the cursor and the line moves right. The last character is lost and can be stored in software.</t>
   </si>
   <si>
     <t xml:space="preserve">'024</t>
@@ -9710,8 +9710,8 @@
   </sheetPr>
   <dimension ref="A1:F258"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10127,7 +10127,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="35" t="s">
         <v>516</v>
       </c>

</xml_diff>